<commit_message>
Updated 40V test data sheets
</commit_message>
<xml_diff>
--- a/Test Data/Verify_40V_Load_On_Changing_CPU_Of_Panel.xlsx
+++ b/Test Data/Verify_40V_Load_On_Changing_CPU_Of_Panel.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jbhosash\Desktop\7th Jan\NGConsys Automation\Test Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B852B20D-C7D7-4BF8-85E0-85BEE551D064}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="5604"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Add Panels" sheetId="6" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="7" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="47">
   <si>
     <t>Color Codes</t>
   </si>
@@ -172,7 +172,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -577,11 +577,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -766,7 +766,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>11</v>
@@ -775,10 +775,10 @@
         <v>27</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="E11" s="6">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="F11" s="10" t="s">
         <v>27</v>
@@ -787,39 +787,39 @@
         <v>27</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="10" t="s">
-        <v>27</v>
+      <c r="C12" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="E12" s="6">
-        <v>6</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="G12" s="10" t="s">
-        <v>27</v>
+        <v>14</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>44</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -830,22 +830,22 @@
         <v>11</v>
       </c>
       <c r="C13" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="6">
+        <v>14</v>
+      </c>
+      <c r="F13" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" s="6">
-        <v>14</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>28</v>
-      </c>
       <c r="G13" s="6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I13" s="12" t="s">
         <v>41</v>
@@ -853,13 +853,13 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>28</v>
+      <c r="C14" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>14</v>
@@ -867,45 +867,16 @@
       <c r="E14" s="6">
         <v>14</v>
       </c>
-      <c r="F14" s="6" t="s">
-        <v>16</v>
+      <c r="F14" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="H14" s="11" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E15" s="6">
-        <v>14</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="H15" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="I15" s="12" t="s">
         <v>38</v>
       </c>
     </row>
@@ -920,7 +891,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>